<commit_message>
Updated with Deduplication of Names Formula
</commit_message>
<xml_diff>
--- a/Named Ranges.xlsx
+++ b/Named Ranges.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$L$10:$L$15</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$L$10:$L$16</definedName>
     <definedName name="_xlnm.Extract" localSheetId="0">Sheet1!$P:$P</definedName>
     <definedName name="WillItems">INDEX(Sheet1!G:G,MATCH("Will",Sheet1!F:F, 0))</definedName>
   </definedNames>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="L9:N15" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="L9:N16" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Item"/>
@@ -415,16 +415,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P20"/>
+  <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="32.28515625" customWidth="1"/>
     <col min="2" max="2" width="24.28515625" customWidth="1"/>
+    <col min="12" max="12" width="16.7109375" customWidth="1"/>
     <col min="16" max="16" width="11" customWidth="1"/>
   </cols>
   <sheetData>
@@ -435,6 +436,20 @@
       <c r="B1" t="s">
         <v>13</v>
       </c>
+      <c r="P1" t="str">
+        <f t="array" ref="P1">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L1))),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J2" t="str">
+        <f t="array" ref="J2">IFERROR(INDEX($L$10:$L$19, MATCH(0, COUNTIF($J$1:J1, $L$10:$L$19), 0)), "")</f>
+        <v>Will</v>
+      </c>
+      <c r="P2" t="str">
+        <f t="array" ref="P2">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L2))),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="e">
@@ -444,17 +459,77 @@
       <c r="B3" t="s">
         <v>12</v>
       </c>
+      <c r="J3" t="str">
+        <f t="array" ref="J3">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J2, $L$10:$L$14), 0)), "")</f>
+        <v>Mark</v>
+      </c>
+      <c r="P3" t="str">
+        <f t="array" ref="P3">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L3))),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="G4" t="str">
         <f>INDEX(M:M,MATCH("Will",L:L, 0))</f>
         <v>ball</v>
       </c>
+      <c r="J4" t="str">
+        <f t="array" ref="J4">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J3, $L$10:$L$14), 0)), "")</f>
+        <v>Gary</v>
+      </c>
+      <c r="P4" t="str">
+        <f t="array" ref="P4">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L4))),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J5" t="str">
+        <f t="array" ref="J5">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J4, $L$10:$L$14), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="P5" t="str">
+        <f t="array" ref="P5">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L5))),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J6" t="str">
+        <f t="array" ref="J6">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J5, $L$10:$L$14), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="P6" t="str">
+        <f t="array" ref="P6">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L6))),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J7" t="str">
+        <f t="array" ref="J7">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J6, $L$10:$L$14), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="P7" t="str">
+        <f t="array" ref="P7">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L7))),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J8" t="str">
+        <f t="array" ref="J8">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J7, $L$10:$L$14), 0)), "")</f>
+        <v/>
+      </c>
+      <c r="P8" t="str">
+        <f t="array" ref="P8">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L8))),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>14</v>
       </c>
+      <c r="J9" t="str">
+        <f t="array" ref="J9">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J8, $L$10:$L$14), 0)), "")</f>
+        <v/>
+      </c>
       <c r="L9" t="s">
         <v>0</v>
       </c>
@@ -464,8 +539,16 @@
       <c r="N9" t="s">
         <v>2</v>
       </c>
+      <c r="P9" t="str">
+        <f t="array" ref="P9">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L9))),"")</f>
+        <v/>
+      </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J10" t="str">
+        <f t="array" ref="J10">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J9, $L$10:$L$14), 0)), "")</f>
+        <v/>
+      </c>
       <c r="L10" t="s">
         <v>3</v>
       </c>
@@ -476,11 +559,15 @@
         <v>2</v>
       </c>
       <c r="P10" t="str">
-        <f>IFERROR(INDEX($L$10:$L$15,MATCH(ROW()-ROW($P$10),$K$10:$K$15,0)),"")</f>
+        <f t="array" ref="P10">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L10))),"")</f>
         <v/>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J11" t="str">
+        <f t="array" ref="J11">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J10, $L$10:$L$14), 0)), "")</f>
+        <v/>
+      </c>
       <c r="L11" t="s">
         <v>3</v>
       </c>
@@ -491,11 +578,15 @@
         <v>3</v>
       </c>
       <c r="P11" t="str">
-        <f t="shared" ref="P11:P20" si="0">IFERROR(INDEX($L$10:$L$15,MATCH(ROW()-ROW($P$10),$K$10:$K$15,0)),"")</f>
+        <f t="array" ref="P11">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L11))),"")</f>
         <v/>
       </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J12" t="str">
+        <f t="array" ref="J12">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J11, $L$10:$L$14), 0)), "")</f>
+        <v/>
+      </c>
       <c r="L12" t="s">
         <v>4</v>
       </c>
@@ -506,7 +597,7 @@
         <v>2</v>
       </c>
       <c r="P12" t="str">
-        <f t="shared" si="0"/>
+        <f t="array" ref="P12">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L12))),"")</f>
         <v/>
       </c>
     </row>
@@ -521,7 +612,7 @@
         <v>3</v>
       </c>
       <c r="P13" t="str">
-        <f t="shared" si="0"/>
+        <f t="array" ref="P13">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L13))),"")</f>
         <v/>
       </c>
     </row>
@@ -536,7 +627,7 @@
         <v>2</v>
       </c>
       <c r="P14" t="str">
-        <f t="shared" si="0"/>
+        <f t="array" ref="P14">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L14))),"")</f>
         <v/>
       </c>
     </row>
@@ -551,37 +642,79 @@
         <v>3</v>
       </c>
       <c r="P15" t="str">
-        <f t="shared" si="0"/>
+        <f t="array" ref="P15">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L15))),"")</f>
         <v/>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="P16" t="str">
-        <f t="shared" si="0"/>
+        <f t="array" ref="P16">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L17))),"")</f>
         <v/>
       </c>
     </row>
     <row r="17" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P17" t="str">
-        <f t="shared" si="0"/>
+        <f t="array" ref="P17">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L18))),"")</f>
         <v/>
       </c>
     </row>
     <row r="18" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P18" t="str">
-        <f t="shared" si="0"/>
+        <f t="array" ref="P18">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L19))),"")</f>
         <v/>
       </c>
     </row>
     <row r="19" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P19" t="str">
-        <f t="shared" si="0"/>
+        <f t="array" ref="P19">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L20))),"")</f>
         <v/>
       </c>
     </row>
     <row r="20" spans="16:16" x14ac:dyDescent="0.25">
       <c r="P20" t="str">
-        <f t="shared" si="0"/>
+        <f t="array" ref="P20">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L21))),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="21" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P21" t="str">
+        <f t="array" ref="P21">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L22))),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="22" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P22" t="str">
+        <f t="array" ref="P22">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L23))),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="23" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P23" t="str">
+        <f t="array" ref="P23">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L24))),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="24" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P24" t="str">
+        <f t="array" ref="P24">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L25))),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="25" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P25" t="str">
+        <f>IFERROR(INDEX($L$10:$L$19,SMALL(IF(ISTEXT($L$10:$L$19),ROW($L$10:$L$19)), ROW(#REF!))),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="26" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P26" t="str">
+        <f>IFERROR(INDEX($L$10:$L$19,SMALL(IF(ISTEXT($L$10:$L$19),ROW($L$10:$L$19)), ROW(#REF!))),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="27" spans="16:16" x14ac:dyDescent="0.25">
+      <c r="P27" t="str">
+        <f>IFERROR(INDEX($L$10:$L$19,SMALL(IF(ISTEXT($L$10:$L$19),ROW($L$10:$L$19)), ROW(#REF!))),"")</f>
         <v/>
       </c>
     </row>

</xml_diff>

<commit_message>
Added 2nd Sheet Reference
</commit_message>
<xml_diff>
--- a/Named Ranges.xlsx
+++ b/Named Ranges.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="17">
   <si>
     <t>Name</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Names</t>
+  </si>
+  <si>
+    <t>Grove</t>
+  </si>
+  <si>
+    <t>Scary</t>
   </si>
 </sst>
 </file>
@@ -119,6 +125,17 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="L9:N16" totalsRowShown="0">
+  <tableColumns count="3">
+    <tableColumn id="1" name="Name"/>
+    <tableColumn id="2" name="Item"/>
+    <tableColumn id="3" name="Value"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleDark3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A1:C8" totalsRowShown="0">
   <tableColumns count="3">
     <tableColumn id="1" name="Name"/>
     <tableColumn id="2" name="Item"/>
@@ -418,7 +435,7 @@
   <dimension ref="A1:P27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="J2" sqref="J2:J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -443,7 +460,7 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J2" t="str">
-        <f t="array" ref="J2">IFERROR(INDEX($L$10:$L$19, MATCH(0, COUNTIF($J$1:J1, $L$10:$L$19), 0)), "")</f>
+        <f t="array" ref="J2">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J1, Sheet2!$A$2:$A$8), 0)), "")</f>
         <v>Will</v>
       </c>
       <c r="P2" t="str">
@@ -460,7 +477,7 @@
         <v>12</v>
       </c>
       <c r="J3" t="str">
-        <f t="array" ref="J3">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J2, $L$10:$L$14), 0)), "")</f>
+        <f t="array" ref="J3">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J2, Sheet2!$A$2:$A$8), 0)), "")</f>
         <v>Mark</v>
       </c>
       <c r="P3" t="str">
@@ -474,8 +491,8 @@
         <v>ball</v>
       </c>
       <c r="J4" t="str">
-        <f t="array" ref="J4">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J3, $L$10:$L$14), 0)), "")</f>
-        <v>Gary</v>
+        <f t="array" ref="J4">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J3, Sheet2!$A$2:$A$8), 0)), "")</f>
+        <v>Grove</v>
       </c>
       <c r="P4" t="str">
         <f t="array" ref="P4">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L4))),"")</f>
@@ -484,8 +501,8 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J5" t="str">
-        <f t="array" ref="J5">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J4, $L$10:$L$14), 0)), "")</f>
-        <v/>
+        <f t="array" ref="J5">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J4, Sheet2!$A$2:$A$8), 0)), "")</f>
+        <v>Gary</v>
       </c>
       <c r="P5" t="str">
         <f t="array" ref="P5">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L5))),"")</f>
@@ -494,8 +511,8 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J6" t="str">
-        <f t="array" ref="J6">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J5, $L$10:$L$14), 0)), "")</f>
-        <v/>
+        <f t="array" ref="J6">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J5, Sheet2!$A$2:$A$8), 0)), "")</f>
+        <v>Scary</v>
       </c>
       <c r="P6" t="str">
         <f t="array" ref="P6">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L6))),"")</f>
@@ -504,7 +521,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J7" t="str">
-        <f t="array" ref="J7">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J6, $L$10:$L$14), 0)), "")</f>
+        <f t="array" ref="J7">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J6, Sheet2!$A$2:$A$8), 0)), "")</f>
         <v/>
       </c>
       <c r="P7" t="str">
@@ -514,7 +531,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J8" t="str">
-        <f t="array" ref="J8">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J7, $L$10:$L$14), 0)), "")</f>
+        <f t="array" ref="J8">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J7, Sheet2!$A$2:$A$8), 0)), "")</f>
         <v/>
       </c>
       <c r="P8" t="str">
@@ -527,7 +544,7 @@
         <v>14</v>
       </c>
       <c r="J9" t="str">
-        <f t="array" ref="J9">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J8, $L$10:$L$14), 0)), "")</f>
+        <f t="array" ref="J9">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J8, Sheet2!$A$2:$A$8), 0)), "")</f>
         <v/>
       </c>
       <c r="L9" t="s">
@@ -546,7 +563,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J10" t="str">
-        <f t="array" ref="J10">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J9, $L$10:$L$14), 0)), "")</f>
+        <f t="array" ref="J10">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J9, Sheet2!$A$2:$A$8), 0)), "")</f>
         <v/>
       </c>
       <c r="L10" t="s">
@@ -565,7 +582,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J11" t="str">
-        <f t="array" ref="J11">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J10, $L$10:$L$14), 0)), "")</f>
+        <f t="array" ref="J11">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J10, Sheet2!$A$2:$A$8), 0)), "")</f>
         <v/>
       </c>
       <c r="L11" t="s">
@@ -584,7 +601,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="J12" t="str">
-        <f t="array" ref="J12">IFERROR(INDEX($L$10:$L$14, MATCH(0, COUNTIF($J$1:J11, $L$10:$L$14), 0)), "")</f>
+        <f t="array" ref="J12">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J11, Sheet2!$A$2:$A$8), 0)), "")</f>
         <v/>
       </c>
       <c r="L12" t="s">
@@ -602,6 +619,10 @@
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J13" t="str">
+        <f t="array" ref="J13">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J12, Sheet2!$A$2:$A$8), 0)), "")</f>
+        <v/>
+      </c>
       <c r="L13" t="s">
         <v>4</v>
       </c>
@@ -617,6 +638,10 @@
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J14" t="str">
+        <f t="array" ref="J14">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J13, Sheet2!$A$2:$A$8), 0)), "")</f>
+        <v/>
+      </c>
       <c r="L14" t="s">
         <v>5</v>
       </c>
@@ -632,6 +657,10 @@
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J15" t="str">
+        <f t="array" ref="J15">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J14, Sheet2!$A$2:$A$8), 0)), "")</f>
+        <v/>
+      </c>
       <c r="L15" t="s">
         <v>5</v>
       </c>
@@ -647,72 +676,100 @@
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J16" t="str">
+        <f t="array" ref="J16">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J15, Sheet2!$A$2:$A$8), 0)), "")</f>
+        <v/>
+      </c>
       <c r="P16" t="str">
         <f t="array" ref="P16">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L17))),"")</f>
         <v/>
       </c>
     </row>
-    <row r="17" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J17" t="str">
+        <f t="array" ref="J17">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J16, Sheet2!$A$2:$A$8), 0)), "")</f>
+        <v/>
+      </c>
       <c r="P17" t="str">
         <f t="array" ref="P17">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L18))),"")</f>
         <v/>
       </c>
     </row>
-    <row r="18" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="18" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J18" t="str">
+        <f t="array" ref="J18">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J17, Sheet2!$A$2:$A$8), 0)), "")</f>
+        <v/>
+      </c>
       <c r="P18" t="str">
         <f t="array" ref="P18">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L19))),"")</f>
         <v/>
       </c>
     </row>
-    <row r="19" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J19" t="str">
+        <f t="array" ref="J19">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J18, Sheet2!$A$2:$A$8), 0)), "")</f>
+        <v/>
+      </c>
       <c r="P19" t="str">
         <f t="array" ref="P19">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L20))),"")</f>
         <v/>
       </c>
     </row>
-    <row r="20" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J20" t="str">
+        <f t="array" ref="J20">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J19, Sheet2!$A$2:$A$8), 0)), "")</f>
+        <v/>
+      </c>
       <c r="P20" t="str">
         <f t="array" ref="P20">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L21))),"")</f>
         <v/>
       </c>
     </row>
-    <row r="21" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J21" t="str">
+        <f t="array" ref="J21">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J20, Sheet2!$A$2:$A$8), 0)), "")</f>
+        <v/>
+      </c>
       <c r="P21" t="str">
         <f t="array" ref="P21">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L22))),"")</f>
         <v/>
       </c>
     </row>
-    <row r="22" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="10:16" x14ac:dyDescent="0.25">
+      <c r="J22" t="str">
+        <f t="array" ref="J22">IFERROR(INDEX(Sheet2!$A$2:$A$8, MATCH(0, COUNTIF($J$1:J21, Sheet2!$A$2:$A$8), 0)), "")</f>
+        <v/>
+      </c>
       <c r="P22" t="str">
         <f t="array" ref="P22">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L23))),"")</f>
         <v/>
       </c>
     </row>
-    <row r="23" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="23" spans="10:16" x14ac:dyDescent="0.25">
       <c r="P23" t="str">
         <f t="array" ref="P23">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L24))),"")</f>
         <v/>
       </c>
     </row>
-    <row r="24" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="10:16" x14ac:dyDescent="0.25">
       <c r="P24" t="str">
         <f t="array" ref="P24">IFERROR(INDEX($L$10:$L$16,SMALL(IF(ISTEXT($L$10:$L$16),ROW($L$1:$L$14)), ROW(L25))),"")</f>
         <v/>
       </c>
     </row>
-    <row r="25" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="10:16" x14ac:dyDescent="0.25">
       <c r="P25" t="str">
         <f>IFERROR(INDEX($L$10:$L$19,SMALL(IF(ISTEXT($L$10:$L$19),ROW($L$10:$L$19)), ROW(#REF!))),"")</f>
         <v/>
       </c>
     </row>
-    <row r="26" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="10:16" x14ac:dyDescent="0.25">
       <c r="P26" t="str">
         <f>IFERROR(INDEX($L$10:$L$19,SMALL(IF(ISTEXT($L$10:$L$19),ROW($L$10:$L$19)), ROW(#REF!))),"")</f>
         <v/>
       </c>
     </row>
-    <row r="27" spans="16:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="10:16" x14ac:dyDescent="0.25">
       <c r="P27" t="str">
         <f>IFERROR(INDEX($L$10:$L$19,SMALL(IF(ISTEXT($L$10:$L$19),ROW($L$10:$L$19)), ROW(#REF!))),"")</f>
         <v/>
@@ -751,13 +808,101 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>